<commit_message>
Improve test coverage for xlsx read
</commit_message>
<xml_diff>
--- a/tests/testRead.xlsx
+++ b/tests/testRead.xlsx
@@ -56,14 +56,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00;[RED]\-#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -123,8 +127,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -145,66 +165,78 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.78"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>1.5</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>43955</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>43955.5626388889</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>